<commit_message>
añadir formaciones y redirecciones de metas
</commit_message>
<xml_diff>
--- a/core/reportes/bases/resultados-operativos.xlsx
+++ b/core/reportes/bases/resultados-operativos.xlsx
@@ -947,6 +947,57 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -956,173 +1007,122 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="17" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2290,8 +2290,8 @@
   </sheetPr>
   <dimension ref="A1:AB104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.42578125" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2317,11 +2317,11 @@
     <row r="2" spans="1:28" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:28" s="2" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="A4" s="82"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2337,55 +2337,55 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:28" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="91"/>
     </row>
     <row r="6" spans="1:28" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="e">
+      <c r="A6" s="90" t="e">
         <f>+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
-      <c r="U6" s="65"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="90"/>
+      <c r="Q6" s="90"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -2406,27 +2406,27 @@
       <c r="A8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="61"/>
-      <c r="P8" s="58" t="s">
+      <c r="B8" s="84"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="59"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="61"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="84"/>
+      <c r="S8" s="85"/>
+      <c r="T8" s="86"/>
       <c r="AA8" s="11" t="s">
         <v>3</v>
       </c>
@@ -2438,25 +2438,25 @@
       <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="68"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="68"/>
-      <c r="T9" s="69"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="93"/>
+      <c r="O9" s="93"/>
+      <c r="P9" s="93"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
+      <c r="S9" s="93"/>
+      <c r="T9" s="94"/>
       <c r="AA9" s="5">
         <v>5</v>
       </c>
@@ -2478,33 +2478,33 @@
     </row>
     <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="62" t="s">
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="62" t="s">
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="63"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="63"/>
-      <c r="V11" s="64"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="88"/>
+      <c r="S11" s="88"/>
+      <c r="T11" s="88"/>
+      <c r="U11" s="88"/>
+      <c r="V11" s="89"/>
     </row>
     <row r="12" spans="1:28" ht="170.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -2611,13 +2611,13 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="74"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="78"/>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:28" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2635,228 +2635,228 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="76"/>
-      <c r="O16" s="77"/>
-      <c r="P16" s="75" t="s">
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="Q16" s="76"/>
-      <c r="R16" s="77"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="81"/>
     </row>
     <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="70"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="55"/>
     </row>
     <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="72"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="70"/>
-      <c r="R18" s="70"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
     </row>
     <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="72"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="70"/>
-      <c r="R19" s="70"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
     </row>
     <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="70"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="70"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
     </row>
     <row r="21" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="71"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
-      <c r="N21" s="72"/>
-      <c r="O21" s="73"/>
-      <c r="P21" s="70"/>
-      <c r="Q21" s="70"/>
-      <c r="R21" s="70"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
     </row>
     <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="72"/>
-      <c r="O22" s="73"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="70"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="55"/>
     </row>
     <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="73"/>
-      <c r="P23" s="70"/>
-      <c r="Q23" s="70"/>
-      <c r="R23" s="70"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
     </row>
     <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="72"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="73"/>
-      <c r="P24" s="70"/>
-      <c r="Q24" s="70"/>
-      <c r="R24" s="70"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
     </row>
     <row r="25" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="71"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="72"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="72"/>
-      <c r="N25" s="72"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="70"/>
-      <c r="Q25" s="70"/>
-      <c r="R25" s="70"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="55"/>
     </row>
     <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="72"/>
-      <c r="O26" s="73"/>
-      <c r="P26" s="70"/>
-      <c r="Q26" s="70"/>
-      <c r="R26" s="70"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
     </row>
     <row r="27" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
@@ -2874,84 +2874,84 @@
       <c r="R27" s="4"/>
     </row>
     <row r="28" spans="1:25" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="79"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="80"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="80"/>
-      <c r="P28" s="80"/>
-      <c r="Q28" s="80"/>
-      <c r="R28" s="80"/>
-      <c r="S28" s="80"/>
-      <c r="T28" s="80"/>
-      <c r="U28" s="80"/>
-      <c r="V28" s="80"/>
-      <c r="W28" s="80"/>
-      <c r="X28" s="81"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="64"/>
+      <c r="P28" s="64"/>
+      <c r="Q28" s="64"/>
+      <c r="R28" s="64"/>
+      <c r="S28" s="64"/>
+      <c r="T28" s="64"/>
+      <c r="U28" s="64"/>
+      <c r="V28" s="64"/>
+      <c r="W28" s="64"/>
+      <c r="X28" s="65"/>
       <c r="Y28" s="34"/>
     </row>
     <row r="29" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="88" t="s">
+      <c r="A29" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="89"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="88" t="s">
+      <c r="B29" s="73"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="90"/>
-      <c r="G29" s="88" t="s">
+      <c r="F29" s="74"/>
+      <c r="G29" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="89"/>
-      <c r="M29" s="82" t="s">
+      <c r="H29" s="73"/>
+      <c r="I29" s="73"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="73"/>
+      <c r="L29" s="73"/>
+      <c r="M29" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="N29" s="83"/>
-      <c r="O29" s="83"/>
-      <c r="P29" s="83"/>
-      <c r="Q29" s="84"/>
-      <c r="R29" s="85" t="s">
+      <c r="N29" s="67"/>
+      <c r="O29" s="67"/>
+      <c r="P29" s="67"/>
+      <c r="Q29" s="68"/>
+      <c r="R29" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="S29" s="86"/>
-      <c r="T29" s="86"/>
-      <c r="U29" s="86"/>
-      <c r="V29" s="86"/>
-      <c r="W29" s="86"/>
-      <c r="X29" s="86"/>
-      <c r="Y29" s="87"/>
+      <c r="S29" s="70"/>
+      <c r="T29" s="70"/>
+      <c r="U29" s="70"/>
+      <c r="V29" s="70"/>
+      <c r="W29" s="70"/>
+      <c r="X29" s="70"/>
+      <c r="Y29" s="71"/>
     </row>
     <row r="30" spans="1:25" ht="164.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="91"/>
-      <c r="B30" s="92"/>
-      <c r="C30" s="92"/>
-      <c r="D30" s="93"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="92"/>
-      <c r="I30" s="92"/>
-      <c r="J30" s="92"/>
-      <c r="K30" s="92"/>
-      <c r="L30" s="92"/>
+      <c r="A30" s="75"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="76"/>
+      <c r="L30" s="76"/>
       <c r="M30" s="35" t="s">
         <v>14</v>
       </c>
@@ -2993,18 +2993,18 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="44"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="61"/>
       <c r="M31" s="33"/>
       <c r="N31" s="33"/>
       <c r="O31" s="33"/>
@@ -3020,18 +3020,18 @@
       <c r="Y31" s="33"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="44"/>
+      <c r="A32" s="59"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="61"/>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
       <c r="O32" s="21"/>
@@ -3047,18 +3047,18 @@
       <c r="Y32" s="21"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="44"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="61"/>
       <c r="M33" s="21"/>
       <c r="N33" s="21"/>
       <c r="O33" s="21"/>
@@ -3074,18 +3074,18 @@
       <c r="Y33" s="21"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="44"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="61"/>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
       <c r="O34" s="21"/>
@@ -3101,18 +3101,18 @@
       <c r="Y34" s="21"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="44"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="61"/>
       <c r="M35" s="21"/>
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
@@ -3128,18 +3128,18 @@
       <c r="Y35" s="21"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="44"/>
+      <c r="A36" s="59"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="60"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="61"/>
       <c r="M36" s="21"/>
       <c r="N36" s="21"/>
       <c r="O36" s="21"/>
@@ -3155,18 +3155,18 @@
       <c r="Y36" s="21"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="44"/>
+      <c r="A37" s="59"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="61"/>
       <c r="M37" s="21"/>
       <c r="N37" s="21"/>
       <c r="O37" s="21"/>
@@ -3182,18 +3182,18 @@
       <c r="Y37" s="21"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="44"/>
+      <c r="A38" s="59"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="61"/>
       <c r="M38" s="21"/>
       <c r="N38" s="21"/>
       <c r="O38" s="21"/>
@@ -3209,29 +3209,29 @@
       <c r="Y38" s="21"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A39" s="94" t="s">
+      <c r="A39" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="94"/>
-      <c r="C39" s="94"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="94"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
-      <c r="K39" s="94"/>
-      <c r="L39" s="94"/>
-      <c r="M39" s="94"/>
-      <c r="N39" s="94"/>
-      <c r="O39" s="94"/>
-      <c r="P39" s="94"/>
-      <c r="Q39" s="94"/>
-      <c r="R39" s="94"/>
-      <c r="S39" s="94"/>
-      <c r="T39" s="94"/>
-      <c r="U39" s="94"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="54"/>
+      <c r="L39" s="54"/>
+      <c r="M39" s="54"/>
+      <c r="N39" s="54"/>
+      <c r="O39" s="54"/>
+      <c r="P39" s="54"/>
+      <c r="Q39" s="54"/>
+      <c r="R39" s="54"/>
+      <c r="S39" s="54"/>
+      <c r="T39" s="54"/>
+      <c r="U39" s="54"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
@@ -3246,16 +3246,16 @@
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="L40" s="9"/>
-      <c r="M40" s="95" t="s">
+      <c r="M40" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="N40" s="95"/>
-      <c r="O40" s="95"/>
-      <c r="P40" s="95"/>
-      <c r="Q40" s="95"/>
-      <c r="R40" s="95"/>
-      <c r="S40" s="95"/>
-      <c r="T40" s="96"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="45"/>
+      <c r="P40" s="45"/>
+      <c r="Q40" s="45"/>
+      <c r="R40" s="45"/>
+      <c r="S40" s="45"/>
+      <c r="T40" s="46"/>
       <c r="U40" s="12"/>
     </row>
     <row r="41" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3278,220 +3278,220 @@
       <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:25" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="97" t="s">
+      <c r="A43" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="98"/>
-      <c r="C43" s="98"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="98"/>
-      <c r="H43" s="98"/>
-      <c r="I43" s="98"/>
-      <c r="J43" s="98"/>
-      <c r="K43" s="98"/>
-      <c r="L43" s="98"/>
-      <c r="M43" s="98"/>
-      <c r="N43" s="98"/>
-      <c r="O43" s="98"/>
-      <c r="P43" s="99" t="s">
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="48"/>
+      <c r="P43" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="Q43" s="100"/>
-      <c r="R43" s="100"/>
-      <c r="S43" s="100"/>
+      <c r="Q43" s="50"/>
+      <c r="R43" s="50"/>
+      <c r="S43" s="50"/>
     </row>
     <row r="44" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
-      <c r="O44" s="49"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="51"/>
-      <c r="R44" s="51"/>
-      <c r="S44" s="52"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="43"/>
+      <c r="M44" s="43"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="44"/>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="52"/>
+      <c r="R44" s="52"/>
+      <c r="S44" s="53"/>
     </row>
     <row r="45" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
-      <c r="M45" s="48"/>
-      <c r="N45" s="48"/>
-      <c r="O45" s="49"/>
-      <c r="P45" s="50"/>
-      <c r="Q45" s="51"/>
-      <c r="R45" s="51"/>
-      <c r="S45" s="52"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="43"/>
+      <c r="O45" s="44"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="52"/>
+      <c r="R45" s="52"/>
+      <c r="S45" s="53"/>
     </row>
     <row r="46" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
-      <c r="O46" s="49"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="51"/>
-      <c r="R46" s="51"/>
-      <c r="S46" s="52"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="43"/>
+      <c r="O46" s="44"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="52"/>
+      <c r="R46" s="52"/>
+      <c r="S46" s="53"/>
     </row>
     <row r="47" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="48"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
-      <c r="M47" s="48"/>
-      <c r="N47" s="48"/>
-      <c r="O47" s="49"/>
-      <c r="P47" s="50"/>
-      <c r="Q47" s="51"/>
-      <c r="R47" s="51"/>
-      <c r="S47" s="52"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+      <c r="N47" s="43"/>
+      <c r="O47" s="44"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="52"/>
+      <c r="R47" s="52"/>
+      <c r="S47" s="53"/>
     </row>
     <row r="48" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="48"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48"/>
-      <c r="M48" s="48"/>
-      <c r="N48" s="48"/>
-      <c r="O48" s="49"/>
-      <c r="P48" s="50"/>
-      <c r="Q48" s="51"/>
-      <c r="R48" s="51"/>
-      <c r="S48" s="52"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
+      <c r="N48" s="43"/>
+      <c r="O48" s="44"/>
+      <c r="P48" s="51"/>
+      <c r="Q48" s="52"/>
+      <c r="R48" s="52"/>
+      <c r="S48" s="53"/>
     </row>
     <row r="49" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-      <c r="O49" s="49"/>
-      <c r="P49" s="50"/>
-      <c r="Q49" s="51"/>
-      <c r="R49" s="51"/>
-      <c r="S49" s="52"/>
+      <c r="A49" s="42"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="43"/>
+      <c r="O49" s="44"/>
+      <c r="P49" s="51"/>
+      <c r="Q49" s="52"/>
+      <c r="R49" s="52"/>
+      <c r="S49" s="53"/>
     </row>
     <row r="50" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="47"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="48"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="48"/>
-      <c r="N50" s="48"/>
-      <c r="O50" s="49"/>
-      <c r="P50" s="50"/>
-      <c r="Q50" s="51"/>
-      <c r="R50" s="51"/>
-      <c r="S50" s="52"/>
+      <c r="A50" s="42"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="43"/>
+      <c r="M50" s="43"/>
+      <c r="N50" s="43"/>
+      <c r="O50" s="44"/>
+      <c r="P50" s="51"/>
+      <c r="Q50" s="52"/>
+      <c r="R50" s="52"/>
+      <c r="S50" s="53"/>
     </row>
     <row r="51" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="48"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="49"/>
-      <c r="P51" s="50"/>
-      <c r="Q51" s="51"/>
-      <c r="R51" s="51"/>
-      <c r="S51" s="52"/>
+      <c r="A51" s="42"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="43"/>
+      <c r="M51" s="43"/>
+      <c r="N51" s="43"/>
+      <c r="O51" s="44"/>
+      <c r="P51" s="51"/>
+      <c r="Q51" s="52"/>
+      <c r="R51" s="52"/>
+      <c r="S51" s="53"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="46"/>
-      <c r="M52" s="46"/>
-      <c r="N52" s="46"/>
-      <c r="O52" s="46"/>
-      <c r="P52" s="46"/>
-      <c r="Q52" s="46"/>
-      <c r="R52" s="46"/>
-      <c r="S52" s="46"/>
+      <c r="B52" s="97"/>
+      <c r="C52" s="97"/>
+      <c r="D52" s="97"/>
+      <c r="E52" s="97"/>
+      <c r="F52" s="97"/>
+      <c r="G52" s="97"/>
+      <c r="H52" s="97"/>
+      <c r="I52" s="97"/>
+      <c r="J52" s="97"/>
+      <c r="K52" s="97"/>
+      <c r="L52" s="97"/>
+      <c r="M52" s="97"/>
+      <c r="N52" s="97"/>
+      <c r="O52" s="97"/>
+      <c r="P52" s="97"/>
+      <c r="Q52" s="97"/>
+      <c r="R52" s="97"/>
+      <c r="S52" s="97"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
@@ -3499,25 +3499,25 @@
       <c r="X52" s="1"/>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A53" s="53"/>
-      <c r="B53" s="54"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="54"/>
-      <c r="I53" s="54"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="54"/>
-      <c r="L53" s="54"/>
-      <c r="M53" s="54"/>
-      <c r="N53" s="54"/>
-      <c r="O53" s="54"/>
-      <c r="P53" s="54"/>
-      <c r="Q53" s="54"/>
-      <c r="R53" s="54"/>
-      <c r="S53" s="55"/>
+      <c r="A53" s="98"/>
+      <c r="B53" s="99"/>
+      <c r="C53" s="99"/>
+      <c r="D53" s="99"/>
+      <c r="E53" s="99"/>
+      <c r="F53" s="99"/>
+      <c r="G53" s="99"/>
+      <c r="H53" s="99"/>
+      <c r="I53" s="99"/>
+      <c r="J53" s="99"/>
+      <c r="K53" s="99"/>
+      <c r="L53" s="99"/>
+      <c r="M53" s="99"/>
+      <c r="N53" s="99"/>
+      <c r="O53" s="99"/>
+      <c r="P53" s="99"/>
+      <c r="Q53" s="99"/>
+      <c r="R53" s="99"/>
+      <c r="S53" s="100"/>
       <c r="T53" s="11"/>
       <c r="U53" s="7"/>
       <c r="V53" s="7"/>
@@ -3525,25 +3525,25 @@
       <c r="X53" s="1"/>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A54" s="53"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="54"/>
-      <c r="F54" s="54"/>
-      <c r="G54" s="54"/>
-      <c r="H54" s="54"/>
-      <c r="I54" s="54"/>
-      <c r="J54" s="54"/>
-      <c r="K54" s="54"/>
-      <c r="L54" s="54"/>
-      <c r="M54" s="54"/>
-      <c r="N54" s="54"/>
-      <c r="O54" s="54"/>
-      <c r="P54" s="54"/>
-      <c r="Q54" s="54"/>
-      <c r="R54" s="54"/>
-      <c r="S54" s="55"/>
+      <c r="A54" s="98"/>
+      <c r="B54" s="99"/>
+      <c r="C54" s="99"/>
+      <c r="D54" s="99"/>
+      <c r="E54" s="99"/>
+      <c r="F54" s="99"/>
+      <c r="G54" s="99"/>
+      <c r="H54" s="99"/>
+      <c r="I54" s="99"/>
+      <c r="J54" s="99"/>
+      <c r="K54" s="99"/>
+      <c r="L54" s="99"/>
+      <c r="M54" s="99"/>
+      <c r="N54" s="99"/>
+      <c r="O54" s="99"/>
+      <c r="P54" s="99"/>
+      <c r="Q54" s="99"/>
+      <c r="R54" s="99"/>
+      <c r="S54" s="100"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
@@ -3551,25 +3551,25 @@
       <c r="X54" s="1"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A55" s="53"/>
-      <c r="B55" s="54"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="54"/>
-      <c r="H55" s="54"/>
-      <c r="I55" s="54"/>
-      <c r="J55" s="54"/>
-      <c r="K55" s="54"/>
-      <c r="L55" s="54"/>
-      <c r="M55" s="54"/>
-      <c r="N55" s="54"/>
-      <c r="O55" s="54"/>
-      <c r="P55" s="54"/>
-      <c r="Q55" s="54"/>
-      <c r="R55" s="54"/>
-      <c r="S55" s="55"/>
+      <c r="A55" s="98"/>
+      <c r="B55" s="99"/>
+      <c r="C55" s="99"/>
+      <c r="D55" s="99"/>
+      <c r="E55" s="99"/>
+      <c r="F55" s="99"/>
+      <c r="G55" s="99"/>
+      <c r="H55" s="99"/>
+      <c r="I55" s="99"/>
+      <c r="J55" s="99"/>
+      <c r="K55" s="99"/>
+      <c r="L55" s="99"/>
+      <c r="M55" s="99"/>
+      <c r="N55" s="99"/>
+      <c r="O55" s="99"/>
+      <c r="P55" s="99"/>
+      <c r="Q55" s="99"/>
+      <c r="R55" s="99"/>
+      <c r="S55" s="100"/>
       <c r="T55" s="11"/>
       <c r="U55" s="7"/>
       <c r="V55" s="7"/>
@@ -3577,25 +3577,25 @@
       <c r="X55" s="1"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A56" s="50"/>
-      <c r="B56" s="51"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="51"/>
-      <c r="G56" s="51"/>
-      <c r="H56" s="51"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="51"/>
-      <c r="K56" s="51"/>
-      <c r="L56" s="51"/>
-      <c r="M56" s="51"/>
-      <c r="N56" s="51"/>
-      <c r="O56" s="51"/>
-      <c r="P56" s="51"/>
-      <c r="Q56" s="51"/>
-      <c r="R56" s="51"/>
-      <c r="S56" s="52"/>
+      <c r="A56" s="42"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="43"/>
+      <c r="M56" s="43"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="43"/>
+      <c r="P56" s="43"/>
+      <c r="Q56" s="43"/>
+      <c r="R56" s="43"/>
+      <c r="S56" s="44"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
@@ -3613,14 +3613,14 @@
       <c r="A58" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D58" s="56" t="s">
+      <c r="D58" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="E58" s="56"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="56"/>
+      <c r="E58" s="95"/>
+      <c r="F58" s="95"/>
+      <c r="G58" s="95"/>
+      <c r="H58" s="95"/>
+      <c r="I58" s="95"/>
       <c r="M58" s="28"/>
       <c r="N58" s="28"/>
       <c r="O58" s="28"/>
@@ -3866,21 +3866,64 @@
   </sortState>
   <dataConsolidate/>
   <mergeCells count="89">
-    <mergeCell ref="A44:O44"/>
-    <mergeCell ref="A51:O51"/>
-    <mergeCell ref="M40:T40"/>
-    <mergeCell ref="A43:O43"/>
-    <mergeCell ref="P43:S43"/>
-    <mergeCell ref="P44:S44"/>
-    <mergeCell ref="P45:S45"/>
-    <mergeCell ref="P46:S46"/>
-    <mergeCell ref="P47:S47"/>
-    <mergeCell ref="A45:O45"/>
-    <mergeCell ref="A46:O46"/>
-    <mergeCell ref="A47:O47"/>
-    <mergeCell ref="P48:S48"/>
-    <mergeCell ref="P49:S49"/>
-    <mergeCell ref="P50:S50"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:L33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A52:S52"/>
+    <mergeCell ref="A48:O48"/>
+    <mergeCell ref="A49:O49"/>
+    <mergeCell ref="A50:O50"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:L34"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:L37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:L38"/>
+    <mergeCell ref="P51:S51"/>
+    <mergeCell ref="A53:S53"/>
+    <mergeCell ref="A54:S54"/>
+    <mergeCell ref="A55:S55"/>
+    <mergeCell ref="A56:S56"/>
+    <mergeCell ref="D58:I58"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B8:O8"/>
+    <mergeCell ref="A6:U6"/>
+    <mergeCell ref="A5:U5"/>
+    <mergeCell ref="B9:T9"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="M11:V11"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="A20:O20"/>
+    <mergeCell ref="A21:O21"/>
+    <mergeCell ref="A22:O22"/>
+    <mergeCell ref="G14:M14"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="A19:O19"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="A16:O16"/>
+    <mergeCell ref="A17:O17"/>
+    <mergeCell ref="A18:O18"/>
+    <mergeCell ref="A28:X28"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:L31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:L32"/>
+    <mergeCell ref="M29:Q29"/>
+    <mergeCell ref="R29:Y29"/>
+    <mergeCell ref="A29:D30"/>
+    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="G29:L30"/>
     <mergeCell ref="A39:U39"/>
     <mergeCell ref="P23:R23"/>
     <mergeCell ref="P24:R24"/>
@@ -3897,64 +3940,21 @@
     <mergeCell ref="G36:L36"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A23:O23"/>
-    <mergeCell ref="A28:X28"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:L31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:L32"/>
-    <mergeCell ref="M29:Q29"/>
-    <mergeCell ref="R29:Y29"/>
-    <mergeCell ref="A29:D30"/>
-    <mergeCell ref="E29:F30"/>
-    <mergeCell ref="G29:L30"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="A20:O20"/>
-    <mergeCell ref="A21:O21"/>
-    <mergeCell ref="A22:O22"/>
-    <mergeCell ref="G14:M14"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="A19:O19"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="A16:O16"/>
-    <mergeCell ref="A17:O17"/>
-    <mergeCell ref="A18:O18"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B8:O8"/>
-    <mergeCell ref="A6:U6"/>
-    <mergeCell ref="A5:U5"/>
-    <mergeCell ref="B9:T9"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="M11:V11"/>
-    <mergeCell ref="A53:S53"/>
-    <mergeCell ref="A54:S54"/>
-    <mergeCell ref="A55:S55"/>
-    <mergeCell ref="A56:S56"/>
-    <mergeCell ref="D58:I58"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:L33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A52:S52"/>
-    <mergeCell ref="A48:O48"/>
-    <mergeCell ref="A49:O49"/>
-    <mergeCell ref="A50:O50"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:L34"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:L37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:L38"/>
-    <mergeCell ref="P51:S51"/>
+    <mergeCell ref="A44:O44"/>
+    <mergeCell ref="A51:O51"/>
+    <mergeCell ref="M40:T40"/>
+    <mergeCell ref="A43:O43"/>
+    <mergeCell ref="P43:S43"/>
+    <mergeCell ref="P44:S44"/>
+    <mergeCell ref="P45:S45"/>
+    <mergeCell ref="P46:S46"/>
+    <mergeCell ref="P47:S47"/>
+    <mergeCell ref="A45:O45"/>
+    <mergeCell ref="A46:O46"/>
+    <mergeCell ref="A47:O47"/>
+    <mergeCell ref="P48:S48"/>
+    <mergeCell ref="P49:S49"/>
+    <mergeCell ref="P50:S50"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
@@ -3981,6 +3981,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100526F55E509A791499B5FB50D930526F2" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="69fc4eb0c2ce4169b40c10b57224ba8e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ebba8a198e9bb40c3eeca6d0bd41257a">
     <xsd:element name="properties">
@@ -4094,15 +4103,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59414364-F888-4581-AEE1-216C77DDE799}">
   <ds:schemaRefs>
@@ -4119,6 +4119,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ADB7CAC-72D0-4757-A2A2-B72C62D84EE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACC3CDD4-36EA-4411-8409-6A388BCD87C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4132,12 +4140,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1ADB7CAC-72D0-4757-A2A2-B72C62D84EE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>